<commit_message>
[feat] basic setting for crawler
</commit_message>
<xml_diff>
--- a/study/store/xlsx/data.xlsx
+++ b/study/store/xlsx/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeonsiwon/Desktop/crawler/study/store/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8747A5-A758-9143-BE6C-E53DCDC8A7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D0270-F3C8-074E-986C-3FB673A64BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16940" activeTab="3" xr2:uid="{D879E8C8-6485-E94A-887D-1A0A658AD990}"/>
   </bookViews>
@@ -1936,7 +1936,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>